<commit_message>
fixed mapping script and added missing attributes
</commit_message>
<xml_diff>
--- a/emx/freeze/rd3_freezeX.xlsx
+++ b/emx/freeze/rd3_freezeX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcruvolo/GitHub/molgenis-solve-rd/emx/freeze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6F7E38-909E-FA4A-AAC9-E9709F96AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC7D72-FA64-E940-845F-FCDF1208514D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-5140" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="267">
   <si>
     <t>name</t>
   </si>
@@ -814,6 +814,15 @@
   </si>
   <si>
     <t>RD3-model_version1.2</t>
+  </si>
+  <si>
+    <t>DateSolved</t>
+  </si>
+  <si>
+    <t>date_solved</t>
+  </si>
+  <si>
+    <t>Date Solved</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1376,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AO85"/>
+  <dimension ref="A1:AO86"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4583,19 +4592,19 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>265</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>264</v>
       </c>
       <c r="C68" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="D68" t="s">
         <v>250</v>
       </c>
       <c r="E68" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G68" t="s">
         <v>58</v>
@@ -4617,12 +4626,6 @@
       </c>
       <c r="N68" t="s">
         <v>27</v>
-      </c>
-      <c r="O68" t="s">
-        <v>138</v>
-      </c>
-      <c r="X68" t="s">
-        <v>6</v>
       </c>
       <c r="Y68" t="s">
         <v>27</v>
@@ -4809,22 +4812,19 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>212</v>
       </c>
       <c r="C73" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D73" t="s">
         <v>250</v>
       </c>
       <c r="E73" t="s">
-        <v>140</v>
-      </c>
-      <c r="F73" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="G73" t="s">
         <v>58</v>
@@ -4838,9 +4838,6 @@
       <c r="J73" t="s">
         <v>27</v>
       </c>
-      <c r="K73" t="s">
-        <v>27</v>
-      </c>
       <c r="L73" t="s">
         <v>27</v>
       </c>
@@ -4849,6 +4846,9 @@
       </c>
       <c r="N73" t="s">
         <v>27</v>
+      </c>
+      <c r="O73" t="s">
+        <v>138</v>
       </c>
       <c r="X73" t="s">
         <v>6</v>
@@ -4859,19 +4859,22 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>76</v>
+        <v>226</v>
       </c>
       <c r="D74" t="s">
         <v>250</v>
       </c>
       <c r="E74" t="s">
-        <v>57</v>
+        <v>140</v>
+      </c>
+      <c r="F74" t="s">
+        <v>74</v>
       </c>
       <c r="G74" t="s">
         <v>58</v>
@@ -4883,6 +4886,9 @@
         <v>58</v>
       </c>
       <c r="J74" t="s">
+        <v>27</v>
+      </c>
+      <c r="K74" t="s">
         <v>27</v>
       </c>
       <c r="L74" t="s">
@@ -4903,43 +4909,40 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="D75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E75" t="s">
         <v>57</v>
       </c>
       <c r="G75" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="H75" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="I75" t="s">
         <v>58</v>
       </c>
       <c r="J75" t="s">
-        <v>58</v>
-      </c>
-      <c r="K75" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="L75" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="M75" t="s">
         <v>27</v>
       </c>
       <c r="N75" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="X75" t="s">
         <v>6</v>
@@ -4950,37 +4953,34 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D76" t="s">
         <v>251</v>
       </c>
       <c r="E76" t="s">
-        <v>73</v>
-      </c>
-      <c r="F76" t="s">
-        <v>250</v>
+        <v>57</v>
       </c>
       <c r="G76" t="s">
         <v>27</v>
       </c>
       <c r="H76" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="I76" t="s">
         <v>58</v>
       </c>
       <c r="J76" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="K76" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="L76" t="s">
         <v>58</v>
@@ -4989,7 +4989,7 @@
         <v>27</v>
       </c>
       <c r="N76" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="X76" t="s">
         <v>6</v>
@@ -5000,22 +5000,25 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="C77" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="D77" t="s">
         <v>251</v>
       </c>
       <c r="E77" t="s">
-        <v>230</v>
+        <v>73</v>
+      </c>
+      <c r="F77" t="s">
+        <v>250</v>
       </c>
       <c r="G77" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="H77" t="s">
         <v>27</v>
@@ -5026,8 +5029,11 @@
       <c r="J77" t="s">
         <v>27</v>
       </c>
+      <c r="K77" t="s">
+        <v>27</v>
+      </c>
       <c r="L77" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="M77" t="s">
         <v>27</v>
@@ -5044,10 +5050,13 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="B78" t="s">
+        <v>228</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D78" t="s">
         <v>251</v>
@@ -5085,10 +5094,10 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D79" t="s">
         <v>251</v>
@@ -5126,22 +5135,16 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>235</v>
-      </c>
-      <c r="B80" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C80" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D80" t="s">
         <v>251</v>
       </c>
       <c r="E80" t="s">
-        <v>73</v>
-      </c>
-      <c r="F80" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="G80" t="s">
         <v>58</v>
@@ -5153,9 +5156,6 @@
         <v>58</v>
       </c>
       <c r="J80" t="s">
-        <v>27</v>
-      </c>
-      <c r="K80" t="s">
         <v>27</v>
       </c>
       <c r="L80" t="s">
@@ -5176,16 +5176,22 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="B81" t="s">
+        <v>235</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D81" t="s">
         <v>251</v>
       </c>
       <c r="E81" t="s">
-        <v>230</v>
+        <v>73</v>
+      </c>
+      <c r="F81" t="s">
+        <v>200</v>
       </c>
       <c r="G81" t="s">
         <v>58</v>
@@ -5197,6 +5203,9 @@
         <v>58</v>
       </c>
       <c r="J81" t="s">
+        <v>27</v>
+      </c>
+      <c r="K81" t="s">
         <v>27</v>
       </c>
       <c r="L81" t="s">
@@ -5217,16 +5226,16 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C82" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D82" t="s">
         <v>251</v>
       </c>
       <c r="E82" t="s">
-        <v>57</v>
+        <v>230</v>
       </c>
       <c r="G82" t="s">
         <v>58</v>
@@ -5258,16 +5267,16 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C83" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D83" t="s">
         <v>251</v>
       </c>
       <c r="E83" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="G83" t="s">
         <v>58</v>
@@ -5299,22 +5308,16 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>70</v>
-      </c>
-      <c r="B84" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="C84" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D84" t="s">
         <v>251</v>
       </c>
       <c r="E84" t="s">
-        <v>140</v>
-      </c>
-      <c r="F84" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="G84" t="s">
         <v>58</v>
@@ -5326,9 +5329,6 @@
         <v>58</v>
       </c>
       <c r="J84" t="s">
-        <v>27</v>
-      </c>
-      <c r="K84" t="s">
         <v>27</v>
       </c>
       <c r="L84" t="s">
@@ -5349,45 +5349,95 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C85" t="s">
-        <v>76</v>
+        <v>226</v>
       </c>
       <c r="D85" t="s">
         <v>251</v>
       </c>
       <c r="E85" t="s">
+        <v>140</v>
+      </c>
+      <c r="F85" t="s">
+        <v>74</v>
+      </c>
+      <c r="G85" t="s">
+        <v>58</v>
+      </c>
+      <c r="H85" t="s">
+        <v>27</v>
+      </c>
+      <c r="I85" t="s">
+        <v>58</v>
+      </c>
+      <c r="J85" t="s">
+        <v>27</v>
+      </c>
+      <c r="K85" t="s">
+        <v>27</v>
+      </c>
+      <c r="L85" t="s">
+        <v>27</v>
+      </c>
+      <c r="M85" t="s">
+        <v>27</v>
+      </c>
+      <c r="N85" t="s">
+        <v>27</v>
+      </c>
+      <c r="X85" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" t="s">
+        <v>76</v>
+      </c>
+      <c r="D86" t="s">
+        <v>251</v>
+      </c>
+      <c r="E86" t="s">
         <v>57</v>
       </c>
-      <c r="G85" t="s">
-        <v>58</v>
-      </c>
-      <c r="H85" t="s">
-        <v>27</v>
-      </c>
-      <c r="I85" t="s">
-        <v>58</v>
-      </c>
-      <c r="J85" t="s">
-        <v>27</v>
-      </c>
-      <c r="L85" t="s">
-        <v>27</v>
-      </c>
-      <c r="M85" t="s">
-        <v>27</v>
-      </c>
-      <c r="N85" t="s">
-        <v>27</v>
-      </c>
-      <c r="X85" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y85" t="s">
+      <c r="G86" t="s">
+        <v>58</v>
+      </c>
+      <c r="H86" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" t="s">
+        <v>58</v>
+      </c>
+      <c r="J86" t="s">
+        <v>27</v>
+      </c>
+      <c r="L86" t="s">
+        <v>27</v>
+      </c>
+      <c r="M86" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" t="s">
+        <v>27</v>
+      </c>
+      <c r="X86" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y86" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
init rd3 freeze yaml and config
</commit_message>
<xml_diff>
--- a/emx/freeze/rd3_freezeX.xlsx
+++ b/emx/freeze/rd3_freezeX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcruvolo/GitHub/molgenis-solve-rd/emx/freeze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3690D8A3-29C9-E54C-9200-E36FABE2B9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972EF1D6-A99E-CE40-B3CD-7DB60269C70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,7 +1278,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1420,7 +1420,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="10" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2097,355 +2097,355 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="X13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="X13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" t="s">
-        <v>58</v>
-      </c>
-      <c r="X14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" t="s">
-        <v>27</v>
-      </c>
-      <c r="X15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" t="s">
-        <v>27</v>
-      </c>
-      <c r="M16" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" t="s">
-        <v>27</v>
-      </c>
-      <c r="X16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="G16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G17" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" t="s">
-        <v>27</v>
-      </c>
-      <c r="X17" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G18" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" t="s">
-        <v>27</v>
-      </c>
-      <c r="X18" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>27</v>
-      </c>
-      <c r="M19" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" t="s">
-        <v>27</v>
-      </c>
-      <c r="X19" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" t="s">
-        <v>27</v>
-      </c>
-      <c r="X20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>